<commit_message>
Updating genes and adding Human genes
</commit_message>
<xml_diff>
--- a/scripts/Elf.xlsx
+++ b/scripts/Elf.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19080" tabRatio="500" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19080" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="15" r:id="rId1"/>
@@ -2628,7 +2628,7 @@
         <v>0.1</v>
       </c>
       <c r="C70" s="9" t="str">
-        <f t="shared" ref="C70:C101" si="2">IF(B70&gt;=1, "common", "rare")</f>
+        <f t="shared" ref="C70:C88" si="2">IF(B70&gt;=1, "common", "rare")</f>
         <v>rare</v>
       </c>
       <c r="D70" s="10"/>
@@ -3361,7 +3361,7 @@
         <v>0.1</v>
       </c>
       <c r="C38" s="9" t="str">
-        <f t="shared" ref="C38:C69" si="1">IF(B38&gt;=1, "common", "rare")</f>
+        <f t="shared" ref="C38:C54" si="1">IF(B38&gt;=1, "common", "rare")</f>
         <v>rare</v>
       </c>
       <c r="D38" s="7"/>
@@ -4067,7 +4067,7 @@
         <v>0.1</v>
       </c>
       <c r="C38" s="9" t="str">
-        <f t="shared" ref="C38:C69" si="1">IF(B38&gt;=1, "common", "rare")</f>
+        <f t="shared" ref="C38:C61" si="1">IF(B38&gt;=1, "common", "rare")</f>
         <v>rare</v>
       </c>
       <c r="D38" s="2"/>
@@ -4571,7 +4571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -6418,7 +6418,7 @@
         <v>0.1</v>
       </c>
       <c r="C70" s="9" t="str">
-        <f t="shared" ref="C70:C101" si="2">IF(B70&gt;=1, "common", "rare")</f>
+        <f t="shared" ref="C70:C80" si="2">IF(B70&gt;=1, "common", "rare")</f>
         <v>rare</v>
       </c>
       <c r="D70" s="2"/>
@@ -8121,8 +8121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C5"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8181,221 +8181,221 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B6" s="5">
         <v>6</v>
       </c>
       <c r="C6" s="9" t="str">
-        <f t="shared" ref="C6:C36" si="0">IF(B6&gt;=1, "common", "rare")</f>
+        <f>IF(B6&gt;=1, "common", "rare")</f>
         <v>common</v>
       </c>
       <c r="D6" s="7"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B7" s="5">
         <v>5</v>
       </c>
       <c r="C7" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B7&gt;=1, "common", "rare")</f>
         <v>common</v>
       </c>
       <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>167</v>
+        <v>21</v>
       </c>
       <c r="B8" s="5">
         <v>4</v>
       </c>
       <c r="C8" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B8&gt;=1, "common", "rare")</f>
         <v>common</v>
       </c>
       <c r="D8" s="7"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>21</v>
+        <v>168</v>
       </c>
       <c r="B9" s="5">
         <v>3</v>
       </c>
       <c r="C9" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B9&gt;=1, "common", "rare")</f>
         <v>common</v>
       </c>
       <c r="D9" s="7"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="B10" s="5">
         <v>2</v>
       </c>
       <c r="C10" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B10&gt;=1, "common", "rare")</f>
         <v>common</v>
       </c>
       <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B11" s="5">
         <v>1</v>
       </c>
       <c r="C11" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B11&gt;=1, "common", "rare")</f>
         <v>common</v>
       </c>
       <c r="D11" s="7"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>164</v>
+        <v>182</v>
       </c>
       <c r="B12" s="5">
         <v>0.1</v>
       </c>
       <c r="C12" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B12&gt;=1, "common", "rare")</f>
         <v>rare</v>
       </c>
       <c r="D12" s="7"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="B13" s="5">
         <v>0.1</v>
       </c>
       <c r="C13" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B13&gt;=1, "common", "rare")</f>
         <v>rare</v>
       </c>
       <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="B14" s="5">
         <v>0.1</v>
       </c>
       <c r="C14" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B14&gt;=1, "common", "rare")</f>
         <v>rare</v>
       </c>
       <c r="D14" s="7"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B15" s="5">
         <v>0.1</v>
       </c>
       <c r="C15" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B15&gt;=1, "common", "rare")</f>
         <v>rare</v>
       </c>
       <c r="D15" s="7"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
       <c r="B16" s="5">
         <v>0.1</v>
       </c>
       <c r="C16" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B16&gt;=1, "common", "rare")</f>
         <v>rare</v>
       </c>
       <c r="D16" s="7"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="B17" s="5">
         <v>0.1</v>
       </c>
       <c r="C17" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B17&gt;=1, "common", "rare")</f>
         <v>rare</v>
       </c>
       <c r="D17" s="7"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B18" s="5">
         <v>0.1</v>
       </c>
       <c r="C18" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B18&gt;=1, "common", "rare")</f>
         <v>rare</v>
       </c>
       <c r="D18" s="7"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="B19" s="5">
         <v>0.1</v>
       </c>
       <c r="C19" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B19&gt;=1, "common", "rare")</f>
         <v>rare</v>
       </c>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B20" s="5">
         <v>0.1</v>
       </c>
       <c r="C20" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B20&gt;=1, "common", "rare")</f>
         <v>rare</v>
       </c>
       <c r="D20" s="7"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B21" s="5">
         <v>0.1</v>
       </c>
       <c r="C21" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B21&gt;=1, "common", "rare")</f>
         <v>rare</v>
       </c>
       <c r="D21" s="7"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>183</v>
+        <v>157</v>
       </c>
       <c r="B22" s="5">
         <v>0.1</v>
       </c>
       <c r="C22" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B22&gt;=1, "common", "rare")</f>
         <v>rare</v>
       </c>
       <c r="D22" s="7"/>
@@ -8408,7 +8408,7 @@
         <v>0.1</v>
       </c>
       <c r="C23" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B23&gt;=1, "common", "rare")</f>
         <v>rare</v>
       </c>
       <c r="D23" s="7"/>
@@ -8421,7 +8421,7 @@
         <v>0.1</v>
       </c>
       <c r="C24" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B24&gt;=1, "common", "rare")</f>
         <v>rare</v>
       </c>
       <c r="D24" s="7"/>
@@ -8434,7 +8434,7 @@
         <v>0.1</v>
       </c>
       <c r="C25" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B25&gt;=1, "common", "rare")</f>
         <v>rare</v>
       </c>
       <c r="D25" s="7"/>
@@ -8447,7 +8447,7 @@
         <v>0.1</v>
       </c>
       <c r="C26" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B26&gt;=1, "common", "rare")</f>
         <v>rare</v>
       </c>
       <c r="D26" s="7"/>
@@ -8460,7 +8460,7 @@
         <v>0.1</v>
       </c>
       <c r="C27" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B27&gt;=1, "common", "rare")</f>
         <v>rare</v>
       </c>
       <c r="D27" s="7"/>
@@ -8473,7 +8473,7 @@
         <v>0.1</v>
       </c>
       <c r="C28" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B28&gt;=1, "common", "rare")</f>
         <v>rare</v>
       </c>
       <c r="D28" s="7"/>
@@ -8486,7 +8486,7 @@
         <v>0.1</v>
       </c>
       <c r="C29" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B29&gt;=1, "common", "rare")</f>
         <v>rare</v>
       </c>
       <c r="D29" s="7"/>
@@ -8499,7 +8499,7 @@
         <v>0.1</v>
       </c>
       <c r="C30" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B30&gt;=1, "common", "rare")</f>
         <v>rare</v>
       </c>
       <c r="D30" s="7"/>
@@ -8512,7 +8512,7 @@
         <v>0.1</v>
       </c>
       <c r="C31" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B31&gt;=1, "common", "rare")</f>
         <v>rare</v>
       </c>
       <c r="D31" s="7"/>
@@ -8525,7 +8525,7 @@
         <v>0.1</v>
       </c>
       <c r="C32" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B32&gt;=1, "common", "rare")</f>
         <v>rare</v>
       </c>
       <c r="D32" s="7"/>
@@ -8538,7 +8538,7 @@
         <v>0.1</v>
       </c>
       <c r="C33" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B33&gt;=1, "common", "rare")</f>
         <v>rare</v>
       </c>
       <c r="D33" s="2"/>
@@ -8551,7 +8551,7 @@
         <v>0.1</v>
       </c>
       <c r="C34" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B34&gt;=1, "common", "rare")</f>
         <v>rare</v>
       </c>
       <c r="D34" s="2"/>
@@ -8564,7 +8564,7 @@
         <v>0.1</v>
       </c>
       <c r="C35" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B35&gt;=1, "common", "rare")</f>
         <v>rare</v>
       </c>
       <c r="D35" s="2"/>
@@ -8577,14 +8577,14 @@
         <v>0.1</v>
       </c>
       <c r="C36" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B36&gt;=1, "common", "rare")</f>
         <v>rare</v>
       </c>
       <c r="D36" s="2"/>
     </row>
   </sheetData>
   <sortState ref="A6:C36">
-    <sortCondition descending="1" ref="B6"/>
+    <sortCondition descending="1" ref="B27"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>